<commit_message>
modif description HS sensitive unit 1648317b1a9513bc9bd1138a9155c84ec487ccc8
</commit_message>
<xml_diff>
--- a/sd-change-def-ror-healthcareservice-sensitive-unit/ig/StructureDefinition-ror-location.xlsx
+++ b/sd-change-def-ror-healthcareservice-sensitive-unit/ig/StructureDefinition-ror-location.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-19T14:04:14+00:00</t>
+    <t>2026-01-20T13:17:16+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2205,7 +2205,7 @@
 </t>
   </si>
   <si>
-    <t>Organization responsible for provisioning and upkeep</t>
+    <t>Hors périmètre du modèle d'exposition du ROR, ce champ est utilisé dans le cas suivant : le Lieu de Réalisation (Location) n'est rattaché à aucune Offre Opérationnelle (HealthcareService), la Location ne pourra alors être rattachée qu'à un ou des HealthcareServices ayant comme parent cette Organization qui doit obligatoirement être une EG</t>
   </si>
   <si>
     <t>The organization responsible for the provisioning and upkeep of the location.</t>

</xml_diff>